<commit_message>
Changes in Dispose Asset Page Updated Add inventory in Bulk backend and format
</commit_message>
<xml_diff>
--- a/CICTInventory/AddInventory_Format.xlsx
+++ b/CICTInventory/AddInventory_Format.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <r>
       <t xml:space="preserve">Item Category*
@@ -27,7 +27,32 @@
     </r>
   </si>
   <si>
-    <t>Quantity*</t>
+    <r>
+      <t xml:space="preserve">Manufacturer*
+</t>
+    </r>
+    <r>
+      <rPr/>
+      <t>(Please enter
+only
+manufacturers
+in the 
+database)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Item Type
+</t>
+    </r>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">(New/Old)
+</t>
+    </r>
+    <r>
+      <t>Default: New</t>
+    </r>
   </si>
   <si>
     <t>Date of Purchase*</t>
@@ -37,26 +62,10 @@
  charged</t>
   </si>
   <si>
-    <t>Price</t>
-  </si>
-  <si>
     <t>Model*</t>
   </si>
   <si>
-    <t>Manufacturer*</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Serial Nos.*
-</t>
-    </r>
-    <r>
-      <rPr/>
-      <t>(Please enter all the serial nos.
- separated by commas(,).
- Make sure that total number of serial 
-nos. is equal to quantity)</t>
-    </r>
+    <t>Serial No.*</t>
   </si>
   <si>
     <r>
@@ -93,6 +102,15 @@
   <si>
     <t>Vendor</t>
   </si>
+  <si>
+    <t>e-File Number</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Section Of Center</t>
+  </si>
 </sst>
 </file>
 
@@ -101,7 +119,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -113,9 +131,9 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
-    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -131,26 +149,23 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -369,36 +384,37 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="16.86"/>
-    <col customWidth="1" min="3" max="3" width="21.0"/>
-    <col customWidth="1" min="4" max="4" width="17.71"/>
+    <col customWidth="1" min="3" max="3" width="16.86"/>
+    <col customWidth="1" min="4" max="4" width="21.0"/>
+    <col customWidth="1" min="5" max="5" width="17.71"/>
     <col customWidth="1" min="6" max="6" width="27.43"/>
-    <col customWidth="1" min="8" max="8" width="36.14"/>
-    <col customWidth="1" min="9" max="9" width="24.43"/>
-    <col customWidth="1" min="10" max="10" width="22.43"/>
-    <col customWidth="1" min="11" max="11" width="16.29"/>
+    <col customWidth="1" min="7" max="7" width="21.43"/>
+    <col customWidth="1" min="8" max="8" width="24.43"/>
+    <col customWidth="1" min="9" max="9" width="22.43"/>
+    <col customWidth="1" min="10" max="10" width="16.29"/>
+    <col customWidth="1" min="14" max="14" width="18.43"/>
   </cols>
   <sheetData>
     <row r="1" ht="102.0" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -410,40 +426,44 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="M2" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>